<commit_message>
updated charts, charts have some test code for sorting by family commented out, and now show unidentified hits as one data slice in the pies/charts
</commit_message>
<xml_diff>
--- a/merge.xlsx
+++ b/merge.xlsx
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1358,7 +1358,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1436,7 +1436,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1514,7 +1514,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1865,7 +1865,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -2021,7 +2021,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -2060,7 +2060,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -2099,7 +2099,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -2189,13 +2189,13 @@
         <v>15</v>
       </c>
       <c r="H45" t="n">
-        <v>5.100000000000001</v>
+        <v>5.1</v>
       </c>
       <c r="I45" t="n">
         <v>884</v>
       </c>
       <c r="J45" t="n">
-        <v>6.78</v>
+        <v>6.779999999999999</v>
       </c>
       <c r="K45" t="n">
         <v>3</v>
@@ -2216,7 +2216,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -2294,7 +2294,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -2333,7 +2333,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -2372,7 +2372,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -2450,7 +2450,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -2489,7 +2489,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -2528,7 +2528,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -2567,7 +2567,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -2606,7 +2606,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -2645,7 +2645,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -2684,7 +2684,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -2840,7 +2840,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -2879,7 +2879,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -2996,7 +2996,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -3035,7 +3035,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -3152,7 +3152,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -3191,7 +3191,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -3308,7 +3308,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
@@ -3386,7 +3386,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -3425,7 +3425,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -3620,7 +3620,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -3659,7 +3659,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -3698,7 +3698,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -3737,7 +3737,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
@@ -3854,7 +3854,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -3971,7 +3971,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
@@ -4010,7 +4010,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
@@ -4049,7 +4049,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -4088,7 +4088,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -4127,7 +4127,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -4166,7 +4166,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -4205,7 +4205,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -4283,7 +4283,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -4400,7 +4400,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
@@ -4439,7 +4439,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
@@ -4478,7 +4478,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E104" t="n">
         <v>2</v>
@@ -4517,7 +4517,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -4556,7 +4556,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E106" t="n">
         <v>0</v>
@@ -4595,7 +4595,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -4634,7 +4634,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -4673,7 +4673,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -4712,7 +4712,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -4751,7 +4751,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
@@ -4790,7 +4790,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
@@ -4829,7 +4829,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E113" t="n">
         <v>0</v>
@@ -4868,7 +4868,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E115" t="n">
         <v>0</v>
@@ -4946,7 +4946,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E116" t="n">
         <v>0</v>
@@ -4985,7 +4985,7 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>
@@ -5024,7 +5024,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E118" t="n">
         <v>0</v>
@@ -5063,7 +5063,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E119" t="n">
         <v>0</v>
@@ -5141,7 +5141,7 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E121" t="n">
         <v>0</v>
@@ -5180,7 +5180,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E122" t="n">
         <v>0</v>
@@ -5219,7 +5219,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E123" t="n">
         <v>0</v>
@@ -5297,7 +5297,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E125" t="n">
         <v>0</v>
@@ -5336,7 +5336,7 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E126" t="n">
         <v>1</v>
@@ -5375,7 +5375,7 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E127" t="n">
         <v>0</v>
@@ -5414,7 +5414,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E128" t="n">
         <v>0</v>
@@ -5453,7 +5453,7 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E129" t="n">
         <v>0</v>
@@ -5492,7 +5492,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E130" t="n">
         <v>0</v>
@@ -5531,7 +5531,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E131" t="n">
         <v>0</v>
@@ -5570,7 +5570,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E132" t="n">
         <v>0</v>
@@ -5609,7 +5609,7 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E133" t="n">
         <v>0</v>
@@ -5648,7 +5648,7 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E134" t="n">
         <v>0</v>
@@ -5687,7 +5687,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E135" t="n">
         <v>0</v>
@@ -5726,7 +5726,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E136" t="n">
         <v>0</v>
@@ -5765,7 +5765,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E137" t="n">
         <v>0</v>
@@ -5804,7 +5804,7 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E138" t="n">
         <v>0</v>
@@ -5843,7 +5843,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E139" t="n">
         <v>0</v>
@@ -5882,7 +5882,7 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E140" t="n">
         <v>0</v>
@@ -5921,7 +5921,7 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E141" t="n">
         <v>0</v>
@@ -5960,7 +5960,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E142" t="n">
         <v>0</v>
@@ -5999,7 +5999,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E143" t="n">
         <v>0</v>
@@ -6038,7 +6038,7 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E144" t="n">
         <v>0</v>

</xml_diff>